<commit_message>
compiling DiD & adding further control variables
</commit_message>
<xml_diff>
--- a/data/processed/treatment_group.xlsx
+++ b/data/processed/treatment_group.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/paulsharratt/Documents/Hertie/Semester 4/03 - Master's Thesis/thesis_stf/data/processed/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C11E24D-FC0A-8047-BE4A-C57582E1E059}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90BF1A65-BCEC-7C4B-9082-19138CD112A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8400" yWindow="22620" windowWidth="17680" windowHeight="15380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="116">
   <si>
     <t>repo</t>
   </si>
@@ -284,9 +284,6 @@
   <si>
     <t xml:space="preserve">Ruby Central Inc. (RubyGems &amp; Bundler (André))
 </t>
-  </si>
-  <si>
-    <t>Ruby Central Inc. (RubyGems 2023)</t>
   </si>
   <si>
     <t>rustls</t>
@@ -728,10 +725,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I25"/>
+  <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I3" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19:XFD19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -745,7 +742,7 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -1261,28 +1258,28 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="B19" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="C19" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="D19" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="E19">
-        <v>150983</v>
+        <v>151276</v>
       </c>
       <c r="F19" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="G19">
-        <v>668400</v>
+        <v>1557468.48</v>
       </c>
       <c r="H19" s="1">
-        <v>45146</v>
+        <v>45084</v>
       </c>
       <c r="I19" s="1">
         <v>45657</v>
@@ -1290,182 +1287,153 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="B20" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="C20" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="D20" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="E20">
-        <v>151276</v>
+        <v>150828</v>
       </c>
       <c r="F20" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="G20">
-        <v>1557468.48</v>
+        <v>455000</v>
       </c>
       <c r="H20" s="1">
-        <v>45084</v>
+        <v>45183</v>
       </c>
       <c r="I20" s="1">
-        <v>45657</v>
+        <v>45473</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="B21" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="C21" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="D21" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="E21">
-        <v>150828</v>
+        <v>150988</v>
       </c>
       <c r="F21" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="G21">
-        <v>455000</v>
+        <v>454350</v>
       </c>
       <c r="H21" s="1">
-        <v>45183</v>
+        <v>45218</v>
       </c>
       <c r="I21" s="1">
-        <v>45473</v>
+        <v>45657</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="B22" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="C22" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="D22" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="E22">
-        <v>150988</v>
+        <v>151272</v>
       </c>
       <c r="F22" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="G22">
-        <v>454350</v>
+        <v>99060</v>
       </c>
       <c r="H22" s="1">
-        <v>45218</v>
+        <v>45205</v>
       </c>
       <c r="I22" s="1">
-        <v>45657</v>
+        <v>45291</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="B23" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="C23" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="D23" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="E23">
-        <v>151272</v>
+        <v>151251</v>
       </c>
       <c r="F23" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="G23">
-        <v>99060</v>
+        <v>152000</v>
       </c>
       <c r="H23" s="1">
-        <v>45205</v>
+        <v>45209</v>
       </c>
       <c r="I23" s="1">
-        <v>45291</v>
+        <v>45535</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="B24" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="C24" t="s">
-        <v>108</v>
-      </c>
-      <c r="D24" t="s">
-        <v>109</v>
+        <v>112</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>113</v>
       </c>
       <c r="E24">
-        <v>151251</v>
+        <v>150822</v>
       </c>
       <c r="F24" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="G24">
-        <v>152000</v>
+        <v>200000</v>
       </c>
       <c r="H24" s="1">
-        <v>45209</v>
+        <v>44886</v>
       </c>
       <c r="I24" s="1">
-        <v>45535</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>111</v>
-      </c>
-      <c r="B25" t="s">
-        <v>112</v>
-      </c>
-      <c r="C25" t="s">
-        <v>113</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="E25">
-        <v>150822</v>
-      </c>
-      <c r="F25" t="s">
-        <v>115</v>
-      </c>
-      <c r="G25">
-        <v>200000</v>
-      </c>
-      <c r="H25" s="1">
-        <v>44886</v>
-      </c>
-      <c r="I25" s="1">
         <v>45098</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D7" r:id="rId1" xr:uid="{F78DFE50-675E-E746-B229-C7578CD71FEB}"/>
-    <hyperlink ref="D25" r:id="rId2" xr:uid="{798B476E-A932-6D4A-9CA1-1B5A537BC374}"/>
+    <hyperlink ref="D24" r:id="rId2" xr:uid="{798B476E-A932-6D4A-9CA1-1B5A537BC374}"/>
     <hyperlink ref="D6" r:id="rId3" xr:uid="{9C977226-6AA7-8B42-88E6-29E83D294F08}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>